<commit_message>
Se termine informe de configuración
</commit_message>
<xml_diff>
--- a/Documentacion/Product Backlog 1.xlsx
+++ b/Documentacion/Product Backlog 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
@@ -730,33 +730,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -865,6 +838,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1584,8 +1584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,40 +1596,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="65"/>
     </row>
     <row r="2" spans="2:10" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="23"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
     </row>
     <row r="3" spans="2:10" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
     </row>
     <row r="4" spans="2:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="26"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="70"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="71"/>
     </row>
     <row r="5" spans="2:10" ht="18" x14ac:dyDescent="0.25">
       <c r="B5" s="16"/>
@@ -1971,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1984,7 +1984,7 @@
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="53" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.7109375" customWidth="1"/>
@@ -2684,730 +2684,730 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="28"/>
-    </row>
-    <row r="3" spans="1:11" s="32" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="B1" s="19"/>
+    </row>
+    <row r="3" spans="1:11" s="23" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="30" t="s">
+      <c r="H3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="31" t="s">
+      <c r="J3" s="22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
+      <c r="A4" s="24">
         <v>1</v>
       </c>
-      <c r="B4" s="34">
+      <c r="B4" s="25">
         <f>IF(OR(B16="",A4=""),"",B16)</f>
         <v>44452</v>
       </c>
-      <c r="C4" s="33">
+      <c r="C4" s="24">
         <f>IF(A4="","",SUMIF(J$16:J$16,A4,C$16:C$16))</f>
         <v>7</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="25">
         <f>IF(OR(B4="",C4=""),"",B4+C4-1)</f>
         <v>44458</v>
       </c>
-      <c r="E4" s="33">
+      <c r="E4" s="24">
         <v>10</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="24">
         <v>15</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="27">
         <v>44465</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="38">
+      <c r="J4" s="29">
         <f>(F4/E4)</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="33">
+      <c r="A5" s="24">
         <v>2</v>
       </c>
-      <c r="B5" s="34">
+      <c r="B5" s="25">
         <f>IF(A5="","",B4+C4)</f>
         <v>44459</v>
       </c>
-      <c r="C5" s="33">
+      <c r="C5" s="24">
         <f>IF(A5="","",SUMIF(J$16:J$17,A5,C$16:C$17))</f>
         <v>0</v>
       </c>
-      <c r="D5" s="34">
-        <f t="shared" ref="D4:D10" si="0">IF(OR(B5="",C5=""),"",B5+C5-1)</f>
+      <c r="D5" s="25">
+        <f t="shared" ref="D5:D10" si="0">IF(OR(B5="",C5=""),"",B5+C5-1)</f>
         <v>44458</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="24">
         <v>14</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="24">
         <v>15</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="27">
         <v>44465</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="I5" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="J5" s="38">
+      <c r="J5" s="29">
         <f>(F5/E5)</f>
         <v>1.0714285714285714</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
+      <c r="A6" s="24">
         <v>3</v>
       </c>
-      <c r="B6" s="34">
+      <c r="B6" s="25">
         <f>IF(A6="","",B5+C5)</f>
         <v>44459</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="24">
         <f>IF(A6="","",SUMIF(J$16:J$18,A6,C$16:C$18))</f>
         <v>0</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="25">
         <f t="shared" si="0"/>
         <v>44458</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="24">
         <f>IF(A6="","",SUMIF(J$16:J$30,'[1]Release Plan'!A6,E$16:E$30))</f>
         <v>0</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="24">
         <f>IF(A6="","",SUMIF(J$16:J$30,'[1]Release Plan'!A6,F$16:F$30))</f>
         <v>0</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="35"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="26"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="41" t="str">
-        <f t="shared" ref="C4:C10" si="1">IF(A7="","",SUMIF(J$16:J$30,A7,C$16:C$30))</f>
-        <v/>
-      </c>
-      <c r="D7" s="40" t="str">
+      <c r="A7" s="30"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32" t="str">
+        <f t="shared" ref="C7:C10" si="1">IF(A7="","",SUMIF(J$16:J$30,A7,C$16:C$30))</f>
+        <v/>
+      </c>
+      <c r="D7" s="31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E7" s="41" t="str">
+      <c r="E7" s="32" t="str">
         <f>IF(A7="","",SUMIF(J$16:J$30,'[1]Release Plan'!A7,E$16:E$30))</f>
         <v/>
       </c>
-      <c r="F7" s="41"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="44"/>
+      <c r="F7" s="32"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40" t="str">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31" t="str">
         <f>IF(OR(B20="",A8=""),"",B20)</f>
         <v/>
       </c>
-      <c r="C8" s="41" t="str">
+      <c r="C8" s="32" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D8" s="40" t="str">
+      <c r="D8" s="31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E8" s="41" t="str">
+      <c r="E8" s="32" t="str">
         <f>IF(A8="","",SUMIF(J$16:J$30,'[1]Release Plan'!A8,E$16:E$30))</f>
         <v/>
       </c>
-      <c r="F8" s="41"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="45"/>
+      <c r="F8" s="32"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="36"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="41" t="str">
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D9" s="40" t="str">
+      <c r="D9" s="31" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E9" s="41" t="str">
+      <c r="E9" s="32" t="str">
         <f>IF(A9="","",SUMIF(J$16:J$30,'[1]Release Plan'!A9,E$16:E$30))</f>
         <v/>
       </c>
-      <c r="F9" s="41"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="45"/>
+      <c r="F9" s="32"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="36"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="46"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="48" t="str">
+      <c r="A10" s="37"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="D10" s="47" t="str">
+      <c r="D10" s="38" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="E10" s="48" t="str">
+      <c r="E10" s="39" t="str">
         <f>IF(A10="","",SUMIF(J$16:J$30,'[1]Release Plan'!A10,E$16:E$30))</f>
         <v/>
       </c>
-      <c r="F10" s="48"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="52"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="43"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
+      <c r="A11" s="44"/>
     </row>
     <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="32" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:11" s="23" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="J15" s="30" t="s">
+      <c r="J15" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="33">
+      <c r="A16" s="24">
         <v>1</v>
       </c>
-      <c r="B16" s="34">
+      <c r="B16" s="25">
         <v>44452</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="45">
         <v>7</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D16" s="25">
         <v>44465</v>
       </c>
-      <c r="E16" s="33">
+      <c r="E16" s="24">
         <v>10</v>
       </c>
-      <c r="F16" s="33">
+      <c r="F16" s="24">
         <v>15</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H16" s="55">
+      <c r="H16" s="46">
         <v>44465</v>
       </c>
-      <c r="I16" s="56" t="s">
+      <c r="I16" s="47" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="54">
+      <c r="J16" s="45">
         <v>1</v>
       </c>
-      <c r="K16" s="38">
+      <c r="K16" s="29">
         <f>(F16/E16)-1</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="33">
+      <c r="A17" s="24">
         <v>2</v>
       </c>
-      <c r="B17" s="34">
+      <c r="B17" s="25">
         <v>44452</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="45">
         <v>14</v>
       </c>
-      <c r="D17" s="34">
+      <c r="D17" s="25">
         <f>IF(AND(B17&lt;&gt;"",C17&lt;&gt;""),B17+C17-1,"")</f>
         <v>44465</v>
       </c>
-      <c r="E17" s="33">
+      <c r="E17" s="24">
         <v>14</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="24">
         <v>15</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="57">
+      <c r="H17" s="48">
         <v>44465</v>
       </c>
-      <c r="I17" s="56" t="s">
+      <c r="I17" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="J17" s="54">
+      <c r="J17" s="45">
         <v>1</v>
       </c>
-      <c r="K17" s="38">
+      <c r="K17" s="29">
         <f>(F17/E17)-1</f>
         <v>7.1428571428571397E-2</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
+      <c r="A18" s="24">
         <v>3</v>
       </c>
-      <c r="B18" s="34">
+      <c r="B18" s="25">
         <v>44459</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18" s="45">
         <v>14</v>
       </c>
-      <c r="D18" s="34">
+      <c r="D18" s="25">
         <f>IF(AND(B18&lt;&gt;"",C18&lt;&gt;""),B18+C18-1,"")</f>
         <v>44472</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="24">
         <v>23</v>
       </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="35" t="s">
+      <c r="F18" s="24"/>
+      <c r="G18" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="57"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="54">
+      <c r="H18" s="48"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="45">
         <v>1</v>
       </c>
-      <c r="K18" s="38">
+      <c r="K18" s="29">
         <f>(F18/E18)-1</f>
         <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="33">
+      <c r="A19" s="24">
         <v>4</v>
       </c>
-      <c r="B19" s="34">
+      <c r="B19" s="25">
         <v>44466</v>
       </c>
-      <c r="C19" s="54">
+      <c r="C19" s="45">
         <v>14</v>
       </c>
-      <c r="D19" s="34">
+      <c r="D19" s="25">
         <f>IF(AND(B19&lt;&gt;"",C19&lt;&gt;""),B19+C19-1,"")</f>
         <v>44479</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="24">
         <v>6</v>
       </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="35" t="s">
+      <c r="F19" s="24"/>
+      <c r="G19" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="57"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="54">
+      <c r="H19" s="48"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="45">
         <v>2</v>
       </c>
-      <c r="K19" s="38">
+      <c r="K19" s="29">
         <f>(F19/E19)-1</f>
         <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="33">
+      <c r="A20" s="24">
         <v>5</v>
       </c>
-      <c r="B20" s="34">
+      <c r="B20" s="25">
         <v>44473</v>
       </c>
-      <c r="C20" s="54">
+      <c r="C20" s="45">
         <v>7</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="25">
         <f>IF(AND(B20&lt;&gt;"",C20&lt;&gt;""),B20+C20-1,"")</f>
         <v>44479</v>
       </c>
-      <c r="E20" s="33">
+      <c r="E20" s="24">
         <v>0</v>
       </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="35" t="s">
+      <c r="F20" s="24"/>
+      <c r="G20" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="54">
+      <c r="H20" s="48"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="45">
         <v>2</v>
       </c>
-      <c r="K20" s="38" t="e">
+      <c r="K20" s="29" t="e">
         <f>(F20/E20)-1</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="33">
+      <c r="A21" s="24">
         <v>6</v>
       </c>
-      <c r="B21" s="34">
+      <c r="B21" s="25">
         <v>44480</v>
       </c>
-      <c r="C21" s="54">
+      <c r="C21" s="45">
         <v>14</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="25">
         <f>IF(AND(B21&lt;&gt;"",C21&lt;&gt;""),B21+C21-1,"")</f>
         <v>44493</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="24">
         <v>0</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="35" t="s">
+      <c r="F21" s="24"/>
+      <c r="G21" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="57"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="54">
+      <c r="H21" s="48"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="45">
         <v>3</v>
       </c>
-      <c r="K21" s="38"/>
+      <c r="K21" s="29"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="41"/>
-      <c r="B22" s="59" t="str">
-        <f t="shared" ref="B17:B30" si="2">IF(AND(B21&lt;&gt;"",C21&lt;&gt;"",C22&lt;&gt;""),B21+C21,"")</f>
-        <v/>
-      </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="59" t="str">
-        <f t="shared" ref="D16:D30" si="3">IF(AND(B22&lt;&gt;"",C22&lt;&gt;""),B22+C22-1,"")</f>
-        <v/>
-      </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="50" t="str">
+        <f t="shared" ref="B22:B30" si="2">IF(AND(B21&lt;&gt;"",C21&lt;&gt;"",C22&lt;&gt;""),B21+C21,"")</f>
+        <v/>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="50" t="str">
+        <f t="shared" ref="D22:D30" si="3">IF(AND(B22&lt;&gt;"",C22&lt;&gt;""),B22+C22-1,"")</f>
+        <v/>
+      </c>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
       <c r="G22" t="str">
         <f t="shared" ref="G22:G30" si="4">IF(AND(OR(G21="Planned",G21="Ongoing"),C22&lt;&gt;""),"Planned","Unplanned")</f>
         <v>Unplanned</v>
       </c>
-      <c r="H22" s="60"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="44"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="35"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="41" t="str">
+      <c r="A23" s="32" t="str">
         <f>IF(AND(B23&lt;&gt;"",C23&lt;&gt;""),A22+1,"")</f>
         <v/>
       </c>
-      <c r="B23" s="59" t="str">
+      <c r="B23" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="59" t="str">
+      <c r="C23" s="20"/>
+      <c r="D23" s="50" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E23" s="41" t="str">
+      <c r="E23" s="32" t="str">
         <f>IF(A23="","",SUMIF('[2]Product Backlog'!E$5:E$79,'[1]Release Plan'!A23,'[2]Product Backlog'!D$5:D$79))</f>
         <v/>
       </c>
-      <c r="F23" s="41"/>
+      <c r="F23" s="32"/>
       <c r="G23" t="str">
         <f t="shared" si="4"/>
         <v>Unplanned</v>
       </c>
-      <c r="I23" s="63"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="45"/>
+      <c r="I23" s="54"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="36"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="str">
+      <c r="A24" s="32" t="str">
         <f t="shared" ref="A24:A30" si="5">IF(AND(B24&lt;&gt;"",C24&lt;&gt;""),A23+1,"")</f>
         <v/>
       </c>
-      <c r="B24" s="59" t="str">
+      <c r="B24" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="59" t="str">
+      <c r="C24" s="20"/>
+      <c r="D24" s="50" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E24" s="41" t="str">
+      <c r="E24" s="32" t="str">
         <f>IF(A24="","",SUMIF('[2]Product Backlog'!E$5:E$79,'[1]Release Plan'!A24,'[2]Product Backlog'!D$5:D$79))</f>
         <v/>
       </c>
-      <c r="F24" s="41"/>
+      <c r="F24" s="32"/>
       <c r="G24" t="str">
         <f t="shared" si="4"/>
         <v>Unplanned</v>
       </c>
-      <c r="I24" s="63"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="45"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="36"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="str">
+      <c r="A25" s="32" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B25" s="59" t="str">
+      <c r="B25" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="59" t="str">
+      <c r="C25" s="20"/>
+      <c r="D25" s="50" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E25" s="41" t="str">
+      <c r="E25" s="32" t="str">
         <f>IF(A25="","",SUMIF('[2]Product Backlog'!E$5:E$79,'[1]Release Plan'!A25,'[2]Product Backlog'!D$5:D$79))</f>
         <v/>
       </c>
-      <c r="F25" s="41"/>
+      <c r="F25" s="32"/>
       <c r="G25" t="str">
         <f t="shared" si="4"/>
         <v>Unplanned</v>
       </c>
-      <c r="I25" s="63"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="45"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="36"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="str">
+      <c r="A26" s="32" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B26" s="59" t="str">
+      <c r="B26" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="59" t="str">
+      <c r="C26" s="20"/>
+      <c r="D26" s="50" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E26" s="41" t="str">
+      <c r="E26" s="32" t="str">
         <f>IF(A26="","",SUMIF('[2]Product Backlog'!E$5:E$79,'[1]Release Plan'!A26,'[2]Product Backlog'!D$5:D$79))</f>
         <v/>
       </c>
-      <c r="F26" s="41"/>
+      <c r="F26" s="32"/>
       <c r="G26" t="str">
         <f t="shared" si="4"/>
         <v>Unplanned</v>
       </c>
-      <c r="I26" s="63"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="45"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="36"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="41" t="str">
+      <c r="A27" s="32" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B27" s="59" t="str">
+      <c r="B27" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="59" t="str">
+      <c r="C27" s="20"/>
+      <c r="D27" s="50" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E27" s="41" t="str">
+      <c r="E27" s="32" t="str">
         <f>IF(A27="","",SUMIF('[2]Product Backlog'!E$5:E$79,'[1]Release Plan'!A27,'[2]Product Backlog'!D$5:D$79))</f>
         <v/>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="32"/>
       <c r="G27" t="str">
         <f t="shared" si="4"/>
         <v>Unplanned</v>
       </c>
-      <c r="I27" s="63"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="45"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="36"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="41" t="str">
+      <c r="A28" s="32" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B28" s="59" t="str">
+      <c r="B28" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="59" t="str">
+      <c r="C28" s="20"/>
+      <c r="D28" s="50" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E28" s="41" t="str">
+      <c r="E28" s="32" t="str">
         <f>IF(A28="","",SUMIF('[2]Product Backlog'!E$5:E$79,'[1]Release Plan'!A28,'[2]Product Backlog'!D$5:D$79))</f>
         <v/>
       </c>
-      <c r="F28" s="41"/>
+      <c r="F28" s="32"/>
       <c r="G28" t="str">
         <f t="shared" si="4"/>
         <v>Unplanned</v>
       </c>
-      <c r="I28" s="63"/>
-      <c r="J28" s="62"/>
-      <c r="K28" s="45"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="36"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="41" t="str">
+      <c r="A29" s="32" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B29" s="59" t="str">
+      <c r="B29" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="59" t="str">
+      <c r="C29" s="20"/>
+      <c r="D29" s="50" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E29" s="41" t="str">
+      <c r="E29" s="32" t="str">
         <f>IF(A29="","",SUMIF('[2]Product Backlog'!E$5:E$79,'[1]Release Plan'!A29,'[2]Product Backlog'!D$5:D$79))</f>
         <v/>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="32"/>
       <c r="G29" t="str">
         <f t="shared" si="4"/>
         <v>Unplanned</v>
       </c>
-      <c r="I29" s="63"/>
-      <c r="J29" s="62"/>
-      <c r="K29" s="45"/>
+      <c r="I29" s="54"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="36"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="41" t="str">
+      <c r="A30" s="32" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="B30" s="59" t="str">
+      <c r="B30" s="50" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="59" t="str">
+      <c r="C30" s="20"/>
+      <c r="D30" s="50" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="E30" s="41" t="str">
+      <c r="E30" s="32" t="str">
         <f>IF(A30="","",SUMIF('[2]Product Backlog'!E$5:E$79,'[1]Release Plan'!A30,'[2]Product Backlog'!D$5:D$79))</f>
         <v/>
       </c>
-      <c r="F30" s="41"/>
+      <c r="F30" s="32"/>
       <c r="G30" t="str">
         <f t="shared" si="4"/>
         <v>Unplanned</v>
       </c>
-      <c r="I30" s="64"/>
-      <c r="J30" s="65"/>
-      <c r="K30" s="52"/>
+      <c r="I30" s="55"/>
+      <c r="J30" s="56"/>
+      <c r="K30" s="43"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
-      <c r="B31" s="66"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="67" t="s">
+      <c r="A31" s="57"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="71" t="e">
+      <c r="E31" s="62" t="e">
         <f>SUMIF('[2]Product Backlog'!E$5:E$79,"",'[2]Product Backlog'!D$5:D$79)-SUMIF('[2]Product Backlog'!C$5:C$79,"Removed",'[2]Product Backlog'!D$5:D$79)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F31" s="68"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="66"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="57"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D32" s="70" t="s">
+      <c r="D32" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="E32" s="68">
+      <c r="E32" s="59">
         <f>SUM(E16:E30)</f>
         <v>53</v>
       </c>
-      <c r="F32" s="68">
+      <c r="F32" s="59">
         <f>SUM(F16:F30)</f>
         <v>30</v>
       </c>

</xml_diff>